<commit_message>
update to comply with new formatting standard
</commit_message>
<xml_diff>
--- a/sampleout.xlsx
+++ b/sampleout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Event</t>
   </si>
@@ -79,6 +79,7 @@
       <sz val="10"/>
       <name val="Nimbus Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -96,12 +97,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,8 +145,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -160,95 +179,105 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="s">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">SUM(C3:G3)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>1</v>
+      <c r="D4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">SUM(C4:G4)</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>